<commit_message>
Changes to be committed: Dashboard page creation
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb719ey\Desktop\eo-master (2)\eo-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub Ivan Vanko\Documents\Škola\Ing\4. ročník\LS\Elektronické obchodovanie\eo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BB0F29-5279-45B9-9FFD-4A54042D15E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -68,12 +67,18 @@
   </si>
   <si>
     <t>Ešte to domyslim</t>
+  </si>
+  <si>
+    <t>UI - Home</t>
+  </si>
+  <si>
+    <t>Dashboard - overview and charts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -298,7 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,26 +515,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -540,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -554,7 +559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -568,7 +573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -582,7 +587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -596,7 +601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -610,15 +615,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -626,7 +637,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -634,7 +645,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -642,7 +653,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -650,7 +661,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -658,7 +669,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -666,7 +677,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -674,7 +685,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -682,7 +693,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -690,7 +701,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -698,7 +709,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -706,7 +717,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -714,7 +725,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -722,7 +733,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Bid progress migration & agregation
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb719ey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomo/Documents/ae/webApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F1E387-0B53-4468-9243-38810C0C7EA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15247BC8-BE56-EC4F-A3A5-0F85D48171CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -58,9 +58,6 @@
     <t>UI - Bid progress</t>
   </si>
   <si>
-    <t>Auction progress curves by ID</t>
-  </si>
-  <si>
     <t>Radoslav Bardovič</t>
   </si>
   <si>
@@ -70,19 +67,13 @@
     <t>UI - Home</t>
   </si>
   <si>
-    <t>Dashboard - overview and charts</t>
-  </si>
-  <si>
-    <t>Karin Jana Szilárdy</t>
-  </si>
-  <si>
-    <t>Price prediction - Linear regression</t>
-  </si>
-  <si>
-    <t>UI - Linear regression</t>
-  </si>
-  <si>
     <t>Visualization of the last price and number of items in the auction</t>
+  </si>
+  <si>
+    <t>Auction progress visualizaion &amp; filtering by columns and participats agregation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard - overview and charts </t>
   </si>
 </sst>
 </file>
@@ -531,20 +522,20 @@
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="66.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -569,7 +560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -583,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -597,35 +588,35 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -633,27 +624,21 @@
         <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -661,7 +646,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -669,7 +654,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -677,7 +662,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -685,7 +670,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -693,7 +678,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -701,7 +686,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -709,7 +694,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -717,7 +702,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -725,7 +710,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -733,7 +718,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -741,7 +726,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -749,7 +734,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Edit filters to enable choosing multiple values and Replace tasks.xlsx
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb719ey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\FEI\EO\Projekt\eo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6093120-172E-4B56-A627-B3F298779BCA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490D7FAD-3B6F-41FA-8164-32322CC4DC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="2196" windowWidth="15336" windowHeight="8040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Cumulative evolution of volumes in items</t>
+  </si>
+  <si>
+    <t>Patrik Masrna</t>
+  </si>
+  <si>
+    <t>UI - Bid progress filters</t>
+  </si>
+  <si>
+    <t>Edit filters in bid progress to enable choosing multiple values</t>
   </si>
 </sst>
 </file>
@@ -598,20 +607,20 @@
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -622,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -636,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -650,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -664,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -678,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -692,7 +701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -706,7 +715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -720,7 +729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -734,7 +743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -748,7 +757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -762,7 +771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -776,15 +785,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>12</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -792,7 +807,7 @@
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -800,7 +815,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -808,7 +823,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -816,7 +831,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -824,7 +839,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -832,7 +847,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -840,7 +855,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Data translation & tasks edition
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\FEI\EO\Projekt\eo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4_rocnik\LS\EO\eo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3F989C-CD1C-4FAA-9796-58DC6E54E236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305596D6-E71E-4E19-B2A8-E93EBD049823}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -119,15 +119,6 @@
   </si>
   <si>
     <t>Exporting prepare_data.r for faster loading app, loading data in global.r</t>
-  </si>
-  <si>
-    <t>Patrik Masrna</t>
-  </si>
-  <si>
-    <t>Filters in Auctions, Bid progress</t>
-  </si>
-  <si>
-    <t>Enabling to select no value or multiple values for filters</t>
   </si>
 </sst>
 </file>
@@ -613,20 +604,20 @@
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="66.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.453125" customWidth="1"/>
+    <col min="5" max="5" width="66.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -637,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -651,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -665,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -679,7 +670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -693,7 +684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -707,7 +698,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -721,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -735,7 +726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -749,7 +740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -763,7 +754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -777,7 +768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -791,7 +782,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -805,21 +796,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -827,7 +812,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -835,7 +820,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -843,7 +828,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -851,7 +836,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -859,7 +844,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -867,7 +852,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
bid progress finalization & edit tasks
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomo/Documents/ae/webApp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4_rocnik\LS\EO\eoGit2\eo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B231CB6-120F-4447-B62B-1171A480E12D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EA3216-76B1-4E9B-AC06-B9F4698ECD6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -43,9 +43,6 @@
     <t xml:space="preserve">Column names correction, Value trimming\factorization &amp; translation, Missing values replacement </t>
   </si>
   <si>
-    <t>Project architecture, Data tables visualization, Task List</t>
-  </si>
-  <si>
     <t>Jakub Ivan Vanko</t>
   </si>
   <si>
@@ -118,7 +115,28 @@
     <t>Data tables visualizaion</t>
   </si>
   <si>
-    <t>Auction progress visualization &amp; filtering by columns and participats agregation, backup available at: https://coder-mano.shinyapps.io/webapp/</t>
+    <t>Bid progress</t>
+  </si>
+  <si>
+    <t>Lucia Szalonová</t>
+  </si>
+  <si>
+    <t>Visualization of most succesful participants according to type and category of auction.</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Kristián Maťašovský</t>
+  </si>
+  <si>
+    <t>Auction progress visualization &amp; filtering by columns and participats agregation</t>
+  </si>
+  <si>
+    <t>Project architecture, Task List</t>
+  </si>
+  <si>
+    <t>Auction progress &amp; all items data preparation &amp; visualization, data translation</t>
   </si>
 </sst>
 </file>
@@ -604,20 +622,20 @@
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="142" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.5" customWidth="1"/>
-    <col min="5" max="5" width="66.5" customWidth="1"/>
+    <col min="4" max="4" width="39.453125" customWidth="1"/>
+    <col min="5" max="5" width="66.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -628,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -639,10 +657,10 @@
         <v>5</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -656,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -664,13 +682,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -678,141 +696,153 @@
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -820,7 +850,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -828,7 +858,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -836,7 +866,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -844,7 +874,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -852,7 +882,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Cleanup, Finalization,Deploy & Final Touch :)
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb719ey\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomo/Documents/ae/webApp - kópia 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2911C6EC-5370-41BD-BA20-FFF1E78F3C2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17B1F31-150F-4D41-8019-1B54EDFBB006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -34,42 +34,45 @@
     <t>Tomáš Adam</t>
   </si>
   <si>
-    <t>Preprocessing</t>
-  </si>
-  <si>
-    <t>User Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column names correction, Value trimming\factorization &amp; translation, Missing values replacement </t>
+    <t>UI - Bid progress</t>
+  </si>
+  <si>
+    <t>Auction progress visualization &amp; filtering by columns and participats agregation</t>
+  </si>
+  <si>
+    <t>Auction progress &amp; all items data preparation &amp; visualization, data translation</t>
+  </si>
+  <si>
+    <t>Radoslav Bardovič</t>
+  </si>
+  <si>
+    <t>UI - Items</t>
   </si>
   <si>
     <t>Jakub Ivan Vanko</t>
   </si>
   <si>
-    <t>UI - Bid progress</t>
-  </si>
-  <si>
-    <t>Radoslav Bardovič</t>
-  </si>
-  <si>
-    <t>UI - Items</t>
+    <t>Exporting prepare_data.r for faster loading app, loading data in global.r</t>
   </si>
   <si>
     <t xml:space="preserve">Dashboard - overview and charts </t>
   </si>
   <si>
+    <t>App Deployment</t>
+  </si>
+  <si>
+    <t>Application Deployment to Shinyapps.io</t>
+  </si>
+  <si>
     <t>Tomáš Nagy, Peter Smolnický</t>
   </si>
   <si>
+    <t>UI - Overview</t>
+  </si>
+  <si>
     <t>Overall description of spendings and other useful informations about clients</t>
   </si>
   <si>
-    <t>App Deployment</t>
-  </si>
-  <si>
-    <t>Application Deployment to Shinyapps.io</t>
-  </si>
-  <si>
     <t>Andrea Mudrová, Benjamín Čarný</t>
   </si>
   <si>
@@ -79,9 +82,6 @@
     <t>Information about data and their statistics</t>
   </si>
   <si>
-    <t>UI - Overview</t>
-  </si>
-  <si>
     <t>Edita Kišková</t>
   </si>
   <si>
@@ -103,37 +103,40 @@
     <t>Exporting data</t>
   </si>
   <si>
-    <t>Exporting prepare_data.r for faster loading app, loading data in global.r</t>
-  </si>
-  <si>
-    <t>UI - Data</t>
-  </si>
-  <si>
-    <t>Data tables visualizaion</t>
-  </si>
-  <si>
-    <t>Bid progress</t>
-  </si>
-  <si>
     <t>Lucia Szalonová</t>
   </si>
   <si>
+    <t>Kristián Maťašovský</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
     <t>Visualization of most succesful participants according to type and category of auction.</t>
   </si>
   <si>
-    <t>Participants</t>
-  </si>
-  <si>
-    <t>Kristián Maťašovský</t>
-  </si>
-  <si>
-    <t>Auction progress visualization &amp; filtering by columns and participats agregation</t>
-  </si>
-  <si>
-    <t>Project architecture, Task List</t>
-  </si>
-  <si>
-    <t>Auction progress &amp; all items data preparation &amp; visualization, data translation</t>
+    <t>User Interface &amp; App deployment</t>
+  </si>
+  <si>
+    <t>Major debuging &amp; Final cleanup</t>
+  </si>
+  <si>
+    <t>UI - Data &amp; Task List</t>
+  </si>
+  <si>
+    <t>Data tables &amp; Tasks visualizaion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column names correction, Value trimming \ factorization &amp; translation, Missing values replacement </t>
+  </si>
+  <si>
+    <t>Data Preprocessing</t>
+  </si>
+  <si>
+    <t>UI - Bid progress &amp; Data Preprocessing</t>
+  </si>
+  <si>
+    <t>Project architecture, Repository maintaining, Major Final debuging &amp; cleanup, App finalization &amp; deployment</t>
   </si>
   <si>
     <t>Cumulative evolution of volumes and past price in items</t>
@@ -392,16 +395,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -622,20 +625,20 @@
   </sheetPr>
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="39.44140625" customWidth="1"/>
-    <col min="5" max="5" width="66.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="66.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -646,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -654,27 +657,27 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -682,13 +685,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -696,83 +699,83 @@
         <v>3</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -786,7 +789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -800,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -811,46 +814,52 @@
         <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -858,7 +867,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -866,7 +875,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -874,7 +883,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -882,7 +891,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="1">
         <v>20</v>
       </c>

</xml_diff>